<commit_message>
added xfinity cookie logic
</commit_message>
<xml_diff>
--- a/NewsID.xlsx
+++ b/NewsID.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="233">
   <si>
     <t>template</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>16903222</t>
+  </si>
+  <si>
+    <t>Dupont</t>
+  </si>
+  <si>
+    <t>102994066</t>
   </si>
 </sst>
 </file>
@@ -1915,7 +1921,14 @@
         <v>230</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>